<commit_message>
update to try logic
</commit_message>
<xml_diff>
--- a/pointtable_boys.xlsx
+++ b/pointtable_boys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCland\Desktop\mora9s-hockey-tournament\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B2C79F-8E62-45C2-8EB9-EB62D7B39231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D602295-4F5A-4456-82F0-82815E8AEE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="252" yWindow="0" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -469,7 +469,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,16 +552,16 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -571,7 +571,7 @@
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I11" si="0">(C3*3)+(D3*1)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J3" t="s">
         <v>17</v>
@@ -594,13 +594,13 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
@@ -618,10 +618,10 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -630,14 +630,14 @@
         <v>5</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J5" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
change penalty points type to number
</commit_message>
<xml_diff>
--- a/pointtable_boys.xlsx
+++ b/pointtable_boys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCland\Desktop\mora9s-hockey-tournament\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70077D3B-8AC2-4385-8190-DBD215FF71B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8720E4B-7811-4947-8BC3-F4457B32C0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="252" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,11 +144,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,14 +460,15 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
     <col min="6" max="6" width="15.5546875" customWidth="1"/>
-    <col min="7" max="8" width="16.21875" customWidth="1"/>
+    <col min="7" max="7" width="16.21875" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -488,7 +493,7 @@
       <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -520,7 +525,7 @@
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>0</v>
       </c>
       <c r="I2">
@@ -553,7 +558,7 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>0</v>
       </c>
       <c r="I3">
@@ -586,7 +591,7 @@
       <c r="G4">
         <v>2</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <v>-6</v>
       </c>
       <c r="I4">
@@ -619,7 +624,7 @@
       <c r="G5">
         <v>2</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="3">
         <v>-3</v>
       </c>
       <c r="I5">
@@ -652,7 +657,7 @@
       <c r="G6">
         <v>3</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="3">
         <v>0</v>
       </c>
       <c r="I6">
@@ -685,7 +690,7 @@
       <c r="G7">
         <v>1</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="3">
         <v>0</v>
       </c>
       <c r="I7">
@@ -718,7 +723,7 @@
       <c r="G8">
         <v>2</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="3">
         <v>0</v>
       </c>
       <c r="I8">
@@ -751,7 +756,7 @@
       <c r="G9">
         <v>4</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="3">
         <v>0</v>
       </c>
       <c r="I9">
@@ -784,7 +789,7 @@
       <c r="G10">
         <v>6</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="3">
         <v>0</v>
       </c>
       <c r="I10">
@@ -817,7 +822,7 @@
       <c r="G11">
         <v>4</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="3">
         <v>0</v>
       </c>
       <c r="I11">
@@ -830,5 +835,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
boys point table final
</commit_message>
<xml_diff>
--- a/pointtable_boys.xlsx
+++ b/pointtable_boys.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCland\Desktop\mora9s-hockey-tournament\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B00440-5D3D-4219-A1C7-8260EE90D9A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F66BCB7-C9C9-466C-B0E5-CD9BDBC23FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12" yWindow="0" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,36 +43,6 @@
     <t>Group</t>
   </si>
   <si>
-    <t>Team A</t>
-  </si>
-  <si>
-    <t>Team B</t>
-  </si>
-  <si>
-    <t>Team C</t>
-  </si>
-  <si>
-    <t>Team D</t>
-  </si>
-  <si>
-    <t>Team E</t>
-  </si>
-  <si>
-    <t>Team F</t>
-  </si>
-  <si>
-    <t>Team G</t>
-  </si>
-  <si>
-    <t>Team H</t>
-  </si>
-  <si>
-    <t>Team I</t>
-  </si>
-  <si>
-    <t>Team J</t>
-  </si>
-  <si>
     <t>Group A</t>
   </si>
   <si>
@@ -95,6 +65,36 @@
   </si>
   <si>
     <t>Red</t>
+  </si>
+  <si>
+    <t>Mora A</t>
+  </si>
+  <si>
+    <t>Sabra</t>
+  </si>
+  <si>
+    <t>Pera</t>
+  </si>
+  <si>
+    <t>Wayamba</t>
+  </si>
+  <si>
+    <t>Rajarata</t>
+  </si>
+  <si>
+    <t>Mora B</t>
+  </si>
+  <si>
+    <t>Ruhuna</t>
+  </si>
+  <si>
+    <t>Kelani</t>
+  </si>
+  <si>
+    <t>Japura</t>
+  </si>
+  <si>
+    <t>Colombo</t>
   </si>
 </sst>
 </file>
@@ -512,11 +512,12 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
     <col min="6" max="6" width="15.5546875" customWidth="1"/>
     <col min="7" max="7" width="16.21875" customWidth="1"/>
@@ -545,13 +546,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
@@ -560,16 +561,16 @@
         <v>6</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="R1" s="6">
         <v>-1</v>
@@ -577,48 +578,39 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="3">
         <f>+L2*$R$1+M2*$R$2+N2*$R$3</f>
-        <v>-7</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <f>(C2*3)+(D2*1)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="6">
-        <v>5</v>
-      </c>
-      <c r="M2" s="8">
-        <v>1</v>
-      </c>
-      <c r="N2" s="10">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q2" s="13" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="R2" s="8">
         <v>-2</v>
@@ -626,45 +618,39 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" s="3">
         <f t="shared" ref="H3:H11" si="0">+L3*$R$1+M3*$R$2+N3*$R$3</f>
-        <v>-7</v>
+        <v>0</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I11" si="1">(C3*3)+(D3*1)</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="6">
-        <v>1</v>
-      </c>
-      <c r="M3" s="8">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="Q3" s="11" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="R3" s="10">
         <v>-5</v>
@@ -672,139 +658,127 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3">
         <f t="shared" si="0"/>
-        <v>-22</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="6">
-        <v>2</v>
-      </c>
-      <c r="N4" s="10">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H5" s="3">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="6">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H6" s="3">
         <f t="shared" si="0"/>
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" s="8">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="3">
         <f t="shared" si="0"/>
@@ -812,33 +786,33 @@
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H8" s="3">
         <f t="shared" si="0"/>
@@ -846,33 +820,33 @@
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J8" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H9" s="3">
         <f t="shared" si="0"/>
@@ -880,33 +854,33 @@
       </c>
       <c r="I9">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J9" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H10" s="3">
         <f t="shared" si="0"/>
@@ -914,18 +888,18 @@
       </c>
       <c r="I10">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -934,13 +908,13 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" si="0"/>
@@ -951,7 +925,7 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>